<commit_message>
doc: Reset du journal de travail temporaire
</commit_message>
<xml_diff>
--- a/Docs/Journal-de-Travail_Temp.xlsx
+++ b/Docs/Journal-de-Travail_Temp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BILEL\Documents\PlotThatLine\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C264671-F3D8-4D6A-868B-922E98F72F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB7A3AB-6114-432A-A4F1-DF6CA92E2768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -128,153 +128,6 @@
   </si>
   <si>
     <t>30.08.2024  au 01.11.2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Création des user et technical stories </t>
-  </si>
-  <si>
-    <t>Recherche du type de donnée (Voir technical Stories)</t>
-  </si>
-  <si>
-    <t>Explication projet par M.Carrel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Introduction par M.Carel + remplissage de la courde </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily scrum  (revue CDC + US iceScrum) </t>
-  </si>
-  <si>
-    <t>Création d'un graphe (essaie non réussis pour cause de temps car temps perdu pour trouver la librairie nécéssaire)</t>
-  </si>
-  <si>
-    <t>Création du premier graph grâce a ScottPlot (Petit problème rencontrer à cause d'un manque d'appelle dans une fonction)</t>
-  </si>
-  <si>
-    <t>Création de deux nouvelle storie sur iceScrum (Conversion date en jour de la semaine + Graphe à multiple ligne)</t>
-  </si>
-  <si>
-    <t>Création d'une méthode qui convertis une date en jour de la semaine</t>
-  </si>
-  <si>
-    <t>Tentative d'afficher un string sur l'axe x avec Scottplot</t>
-  </si>
-  <si>
-    <t>Tentative d'afficher un string sur l'axe x avec Scottplot réussi (problème rencontrer du a un changement dans la version de la libraire ayant changer le nom de certaine methode beaucoup de recherche ont du être faites)</t>
-  </si>
-  <si>
-    <t>Refactorisation du tableau "nbPoint" en liste (factorisation nécessitant l'ajout d'une methode pour passer les valeur de la liste dans un tableau pour l'affichage du graph)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Refactorisation du code du graphe afin qu'il puisse afficher plusieur équipes </t>
-  </si>
-  <si>
-    <t>Création de la classe team et refactorisation du code afin qu'il utilise la liste des score de la classe team</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Appel a une api oke </t>
-  </si>
-  <si>
-    <t>Absence</t>
-  </si>
-  <si>
-    <t>Discussion avec le prof sur l'evolution du métier</t>
-  </si>
-  <si>
-    <t>Ajout d'un fichier CSV contenant les données des équipes</t>
-  </si>
-  <si>
-    <t>Ajout de la methode getAllTeams qui permet de récupéer toutes les équipe de la nba en lisant le fichier CSV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ajout de la methode getTeamsStats qui permet de récupérer pour chaque équipe NBA leur statistique pour la saison </t>
-  </si>
-  <si>
-    <t>Essaie de conversion de la date en string du CSV en format numéros du jour de la semaine ()</t>
-  </si>
-  <si>
-    <t>Récupération dans une liste d'équipe l'équipe ainsi que son score et le jour du match</t>
-  </si>
-  <si>
-    <t>M.Carrel nous a donné des feedback sur l'avancé des projets (Besoin d'avancer sur la documentation)</t>
-  </si>
-  <si>
-    <t>Fix de la méthode GetTeamStructure (Bug: La séléction des données était éronnée et attribuait le score de l'équipe à domicil si l'équipe jouait à l'extérieur)</t>
-  </si>
-  <si>
-    <t>Feat: Affichage des ligne pour chaque équipe sur le graphe</t>
-  </si>
-  <si>
-    <t>Création US</t>
-  </si>
-  <si>
-    <t>Mise à jour VS</t>
-  </si>
-  <si>
-    <t>Tentative de rendre les legendes cliquable (Non réussite)</t>
-  </si>
-  <si>
-    <t>Feat: Mise en place du filtre par équipe</t>
-  </si>
-  <si>
-    <t>Revue du test pratique avec le prof</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revue/correction des user stories </t>
-  </si>
-  <si>
-    <t>Le prof nous a présenter IceTools</t>
-  </si>
-  <si>
-    <t>Ecriture de l'introduction de l'analyse prélininaire du rapport</t>
-  </si>
-  <si>
-    <t>Ecriture de la partie objectif de l'analyse préliminaire</t>
-  </si>
-  <si>
-    <t>Ecriture de la partie gestion de l'analyse préliminaire</t>
-  </si>
-  <si>
-    <t>Pause</t>
-  </si>
-  <si>
-    <t>Ecriture de la partie domaine de l'analyse/conception</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Refactore: (Graph.cs) changement de la methode button_click() afin de simplement désafficher les scatters plutôt que de les supprimer </t>
-  </si>
-  <si>
-    <t>Refactore: (Form1 conception) création du graph dans la conception du form plutôt que le créer dans le code</t>
-  </si>
-  <si>
-    <t>Refactore: (Graph.cs) Mise en place du flowLayoutPanel dans la conception</t>
-  </si>
-  <si>
-    <t>Doc: (DataSelection.cs) Ajout des commentaires dans la classe DataSelection.cs</t>
-  </si>
-  <si>
-    <t>Refcatore: (Graph.cs) Remplacement des bouton représentant les équipes pour les filtres par des checkBox</t>
-  </si>
-  <si>
-    <t>Chore: (Graph.cs) Ajout des commentaires dans la classe</t>
-  </si>
-  <si>
-    <t>refactore: (Graph.cs) remplacement des tableaux de jour par une liste de tuple (numéros jour de la semaine,  nom du jour)</t>
-  </si>
-  <si>
-    <t>Tentative ajout filtre avec jour</t>
-  </si>
-  <si>
-    <t>Feat: (Graph.cs) ajout des filtre par jour</t>
-  </si>
-  <si>
-    <t>Refactor: (Graph.cs) déplacement de la methode CreateDisableAllTeamsCheckBox(); afin de la mettre dans le constructor</t>
-  </si>
-  <si>
-    <t>Fix: (Graph.cs) re création des checkbox d'équipe a chaque filtre par jour</t>
-  </si>
-  <si>
-    <t>Feat: (Graph.cs) changement du type de ligne en bar si l'utilisateur n'affiche qu'un seul jour</t>
   </si>
 </sst>
 </file>
@@ -1206,19 +1059,19 @@
                 <c:formatCode>hh\ "h"\ mm\ "min"</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>4.1666666666666664E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.73263888888888884</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.5972222222222224E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.125E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1227,7 +1080,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.9444444444444448E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2139,8 +1992,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F59" sqref="F59"/>
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -2193,7 +2046,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>1 jours 3 heurs 35 minutes</v>
+        <v>0 jours 0 heurs 0 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2208,15 +2061,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="23">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>840</v>
+        <v>0</v>
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>815</v>
+        <v>0</v>
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>1655</v>
+        <v>0</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2251,43 +2104,27 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A7" s="14">
+      <c r="A7" s="14" t="str">
         <f>IF(ISBLANK(B7),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B7))</f>
-        <v>35</v>
-      </c>
-      <c r="B7" s="43">
-        <v>45534</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B7" s="43"/>
       <c r="C7" s="44"/>
-      <c r="D7" s="45">
-        <v>15</v>
-      </c>
-      <c r="E7" s="46" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="37" t="s">
-        <v>29</v>
-      </c>
+      <c r="D7" s="45"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="37"/>
       <c r="G7" s="15"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A8" s="8">
+      <c r="A8" s="8" t="str">
         <f>IF(ISBLANK(B8),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B8))</f>
-        <v>35</v>
-      </c>
-      <c r="B8" s="47">
-        <v>45534</v>
-      </c>
-      <c r="C8" s="48">
-        <v>1</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B8" s="47"/>
+      <c r="C8" s="48"/>
       <c r="D8" s="49"/>
-      <c r="E8" s="50" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="37" t="s">
-        <v>30</v>
-      </c>
+      <c r="E8" s="50"/>
+      <c r="F8" s="37"/>
       <c r="G8" s="16"/>
       <c r="M8" t="s">
         <v>3</v>
@@ -2300,25 +2137,15 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A9" s="17">
+      <c r="A9" s="17" t="str">
         <f>IF(ISBLANK(B9),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B9))</f>
-        <v>35</v>
-      </c>
-      <c r="B9" s="51">
-        <v>45534</v>
-      </c>
-      <c r="C9" s="52">
-        <v>1</v>
-      </c>
-      <c r="D9" s="53">
-        <v>30</v>
-      </c>
-      <c r="E9" s="54" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="37" t="s">
-        <v>31</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B9" s="51"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="37"/>
       <c r="G9" s="18"/>
       <c r="M9" t="s">
         <v>4</v>
@@ -2330,24 +2157,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A10" s="8">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="A10" s="8" t="str">
         <f>IF(ISBLANK(B10),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B10))</f>
-        <v>35</v>
-      </c>
-      <c r="B10" s="47">
-        <v>45534</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B10" s="47"/>
       <c r="C10" s="48"/>
-      <c r="D10" s="49">
-        <v>10</v>
-      </c>
-      <c r="E10" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" s="37" t="s">
-        <v>34</v>
-      </c>
+      <c r="D10" s="49"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="37"/>
       <c r="G10" s="16"/>
       <c r="M10" t="s">
         <v>5</v>
@@ -2360,23 +2179,15 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A11" s="17">
+      <c r="A11" s="17" t="str">
         <f>IF(ISBLANK(B11),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B11))</f>
-        <v>36</v>
-      </c>
-      <c r="B11" s="51">
-        <v>45541</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B11" s="51"/>
       <c r="C11" s="52"/>
-      <c r="D11" s="53">
-        <v>15</v>
-      </c>
-      <c r="E11" s="54" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="37" t="s">
-        <v>32</v>
-      </c>
+      <c r="D11" s="53"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="37"/>
       <c r="G11" s="18"/>
       <c r="M11" t="s">
         <v>6</v>
@@ -2389,23 +2200,15 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A12" s="8">
+      <c r="A12" s="8" t="str">
         <f>IF(ISBLANK(B12),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B12))</f>
-        <v>36</v>
-      </c>
-      <c r="B12" s="47">
-        <v>45541</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B12" s="47"/>
       <c r="C12" s="48"/>
-      <c r="D12" s="49">
-        <v>5</v>
-      </c>
-      <c r="E12" s="50" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" s="37" t="s">
-        <v>33</v>
-      </c>
+      <c r="D12" s="49"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="37"/>
       <c r="G12" s="16"/>
       <c r="M12" t="s">
         <v>7</v>
@@ -2417,24 +2220,16 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A13" s="17">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="A13" s="17" t="str">
         <f>IF(ISBLANK(B13),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B13))</f>
-        <v>36</v>
-      </c>
-      <c r="B13" s="51">
-        <v>45541</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B13" s="51"/>
       <c r="C13" s="52"/>
-      <c r="D13" s="53">
-        <v>50</v>
-      </c>
-      <c r="E13" s="54" t="s">
-        <v>4</v>
-      </c>
-      <c r="F13" s="37" t="s">
-        <v>35</v>
-      </c>
+      <c r="D13" s="53"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="37"/>
       <c r="G13" s="18"/>
       <c r="M13" t="s">
         <v>8</v>
@@ -2446,24 +2241,16 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A14" s="8">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="A14" s="8" t="str">
         <f>IF(ISBLANK(B14),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B14))</f>
-        <v>36</v>
-      </c>
-      <c r="B14" s="47">
-        <v>45541</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B14" s="47"/>
       <c r="C14" s="48"/>
-      <c r="D14" s="49">
-        <v>15</v>
-      </c>
-      <c r="E14" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14" s="37" t="s">
-        <v>36</v>
-      </c>
+      <c r="D14" s="49"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="37"/>
       <c r="G14" s="16"/>
       <c r="M14" t="s">
         <v>21</v>
@@ -2476,23 +2263,15 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A15" s="17">
+      <c r="A15" s="17" t="str">
         <f>IF(ISBLANK(B15),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B15))</f>
-        <v>36</v>
-      </c>
-      <c r="B15" s="51">
-        <v>45541</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B15" s="51"/>
       <c r="C15" s="52"/>
-      <c r="D15" s="53">
-        <v>15</v>
-      </c>
-      <c r="E15" s="54" t="s">
-        <v>4</v>
-      </c>
-      <c r="F15" s="37" t="s">
-        <v>37</v>
-      </c>
+      <c r="D15" s="53"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="37"/>
       <c r="G15" s="18"/>
       <c r="M15" t="s">
         <v>22</v>
@@ -2505,817 +2284,495 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A16" s="8">
+      <c r="A16" s="8" t="str">
         <f>IF(ISBLANK(B16),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B16))</f>
-        <v>36</v>
-      </c>
-      <c r="B16" s="47">
-        <v>45541</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B16" s="47"/>
       <c r="C16" s="48"/>
-      <c r="D16" s="49">
-        <v>20</v>
-      </c>
-      <c r="E16" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="F16" s="37" t="s">
-        <v>38</v>
-      </c>
+      <c r="D16" s="49"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="37"/>
       <c r="G16" s="16"/>
       <c r="O16">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="47.25" x14ac:dyDescent="0.5">
-      <c r="A17" s="17">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="A17" s="17" t="str">
         <f>IF(ISBLANK(B17),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B17))</f>
-        <v>37</v>
-      </c>
-      <c r="B17" s="51">
-        <v>45548</v>
-      </c>
-      <c r="C17" s="52">
-        <v>1</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B17" s="51"/>
+      <c r="C17" s="52"/>
       <c r="D17" s="53"/>
-      <c r="E17" s="54" t="s">
-        <v>4</v>
-      </c>
-      <c r="F17" s="37" t="s">
-        <v>39</v>
-      </c>
+      <c r="E17" s="54"/>
+      <c r="F17" s="37"/>
       <c r="G17" s="18"/>
       <c r="O17">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A18" s="8">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="A18" s="8" t="str">
         <f>IF(ISBLANK(B18),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B18))</f>
-        <v>37</v>
-      </c>
-      <c r="B18" s="47">
-        <v>45548</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B18" s="47"/>
       <c r="C18" s="48"/>
-      <c r="D18" s="49">
-        <v>15</v>
-      </c>
-      <c r="E18" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="F18" s="37" t="s">
-        <v>40</v>
-      </c>
+      <c r="D18" s="49"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="37"/>
       <c r="G18" s="16"/>
       <c r="O18">
         <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A19" s="17">
+      <c r="A19" s="17" t="str">
         <f>IF(ISBLANK(B19),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B19))</f>
-        <v>37</v>
-      </c>
-      <c r="B19" s="51">
-        <v>45548</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B19" s="51"/>
       <c r="C19" s="52"/>
-      <c r="D19" s="53">
-        <v>30</v>
-      </c>
-      <c r="E19" s="54" t="s">
-        <v>4</v>
-      </c>
-      <c r="F19" s="37" t="s">
-        <v>41</v>
-      </c>
+      <c r="D19" s="53"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="37"/>
       <c r="G19" s="18"/>
       <c r="O19">
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A20" s="8">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="A20" s="8" t="str">
         <f>IF(ISBLANK(B20),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B20))</f>
-        <v>37</v>
-      </c>
-      <c r="B20" s="47">
-        <v>45548</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B20" s="47"/>
       <c r="C20" s="48"/>
-      <c r="D20" s="49">
-        <v>10</v>
-      </c>
-      <c r="E20" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="F20" s="37" t="s">
-        <v>42</v>
-      </c>
+      <c r="D20" s="49"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="37"/>
       <c r="G20" s="16"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A21" s="17">
+      <c r="A21" s="17" t="str">
         <f>IF(ISBLANK(B21),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B21))</f>
-        <v>37</v>
-      </c>
-      <c r="B21" s="51">
-        <v>45548</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B21" s="51"/>
       <c r="C21" s="52"/>
-      <c r="D21" s="53">
-        <v>40</v>
-      </c>
-      <c r="E21" s="54" t="s">
-        <v>4</v>
-      </c>
-      <c r="F21" s="37" t="s">
-        <v>43</v>
-      </c>
+      <c r="D21" s="53"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="37"/>
       <c r="G21" s="18"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A22" s="8">
+      <c r="A22" s="8" t="str">
         <f>IF(ISBLANK(B22),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B22))</f>
-        <v>38</v>
-      </c>
-      <c r="B22" s="47">
-        <v>45555</v>
-      </c>
-      <c r="C22" s="48">
-        <v>3</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B22" s="47"/>
+      <c r="C22" s="48"/>
       <c r="D22" s="49"/>
-      <c r="E22" s="50" t="s">
-        <v>22</v>
-      </c>
-      <c r="F22" s="37" t="s">
-        <v>44</v>
-      </c>
+      <c r="E22" s="50"/>
+      <c r="F22" s="37"/>
       <c r="G22" s="16"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A23" s="17">
+      <c r="A23" s="17" t="str">
         <f>IF(ISBLANK(B23),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B23))</f>
-        <v>39</v>
-      </c>
-      <c r="B23" s="51">
-        <v>45562</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B23" s="51"/>
       <c r="C23" s="52"/>
-      <c r="D23" s="53">
-        <v>10</v>
-      </c>
-      <c r="E23" s="54" t="s">
-        <v>22</v>
-      </c>
-      <c r="F23" s="37" t="s">
-        <v>45</v>
-      </c>
+      <c r="D23" s="53"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="37"/>
       <c r="G23" s="18"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A24" s="8">
+      <c r="A24" s="8" t="str">
         <f>IF(ISBLANK(B24),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B24))</f>
-        <v>39</v>
-      </c>
-      <c r="B24" s="47">
-        <v>45562</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B24" s="47"/>
       <c r="C24" s="48"/>
-      <c r="D24" s="49">
-        <v>35</v>
-      </c>
-      <c r="E24" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="F24" s="37" t="s">
-        <v>46</v>
-      </c>
+      <c r="D24" s="49"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="37"/>
       <c r="G24" s="16"/>
     </row>
-    <row r="25" spans="1:15" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A25" s="17">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="A25" s="17" t="str">
         <f>IF(ISBLANK(B25),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B25))</f>
-        <v>39</v>
-      </c>
-      <c r="B25" s="51">
-        <v>45562</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B25" s="51"/>
       <c r="C25" s="52"/>
-      <c r="D25" s="53">
-        <v>40</v>
-      </c>
-      <c r="E25" s="54" t="s">
-        <v>4</v>
-      </c>
-      <c r="F25" s="37" t="s">
-        <v>47</v>
-      </c>
+      <c r="D25" s="53"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="37"/>
       <c r="G25" s="18"/>
     </row>
-    <row r="26" spans="1:15" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A26" s="8">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="A26" s="8" t="str">
         <f>IF(ISBLANK(B26),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B26))</f>
-        <v>39</v>
-      </c>
-      <c r="B26" s="47">
-        <v>45562</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B26" s="47"/>
       <c r="C26" s="48"/>
-      <c r="D26" s="49">
-        <v>35</v>
-      </c>
-      <c r="E26" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="F26" s="37" t="s">
-        <v>48</v>
-      </c>
+      <c r="D26" s="49"/>
+      <c r="E26" s="50"/>
+      <c r="F26" s="37"/>
       <c r="G26" s="16"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A27" s="17">
+      <c r="A27" s="17" t="str">
         <f>IF(ISBLANK(B27),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B27))</f>
-        <v>39</v>
-      </c>
-      <c r="B27" s="51">
-        <v>45562</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B27" s="51"/>
       <c r="C27" s="52"/>
-      <c r="D27" s="53">
-        <v>40</v>
-      </c>
-      <c r="E27" s="54" t="s">
-        <v>4</v>
-      </c>
-      <c r="F27" s="37" t="s">
-        <v>49</v>
-      </c>
+      <c r="D27" s="53"/>
+      <c r="E27" s="54"/>
+      <c r="F27" s="37"/>
       <c r="G27" s="18"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A28" s="8">
+      <c r="A28" s="8" t="str">
         <f>IF(ISBLANK(B28),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B28))</f>
-        <v>40</v>
-      </c>
-      <c r="B28" s="47">
-        <v>45568</v>
-      </c>
-      <c r="C28" s="48">
-        <v>1</v>
-      </c>
-      <c r="D28" s="49">
-        <v>15</v>
-      </c>
-      <c r="E28" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="F28" s="36" t="s">
-        <v>50</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B28" s="47"/>
+      <c r="C28" s="48"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="36"/>
       <c r="G28" s="16"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A29" s="17">
+      <c r="A29" s="17" t="str">
         <f>IF(ISBLANK(B29),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B29))</f>
-        <v>40</v>
-      </c>
-      <c r="B29" s="51">
-        <v>45569</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B29" s="51"/>
       <c r="C29" s="52"/>
-      <c r="D29" s="53">
-        <v>15</v>
-      </c>
-      <c r="E29" s="54" t="s">
-        <v>7</v>
-      </c>
-      <c r="F29" s="36" t="s">
-        <v>51</v>
-      </c>
+      <c r="D29" s="53"/>
+      <c r="E29" s="54"/>
+      <c r="F29" s="36"/>
       <c r="G29" s="18"/>
     </row>
-    <row r="30" spans="1:15" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A30" s="8">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.5">
+      <c r="A30" s="8" t="str">
         <f>IF(ISBLANK(B30),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B30))</f>
-        <v>40</v>
-      </c>
-      <c r="B30" s="47">
-        <v>45569</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B30" s="47"/>
       <c r="C30" s="48"/>
-      <c r="D30" s="49">
-        <v>10</v>
-      </c>
-      <c r="E30" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="F30" s="37" t="s">
-        <v>52</v>
-      </c>
+      <c r="D30" s="49"/>
+      <c r="E30" s="50"/>
+      <c r="F30" s="37"/>
       <c r="G30" s="16"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A31" s="17">
+      <c r="A31" s="17" t="str">
         <f>IF(ISBLANK(B31),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B31))</f>
-        <v>40</v>
-      </c>
-      <c r="B31" s="51">
-        <v>45569</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B31" s="51"/>
       <c r="C31" s="52"/>
-      <c r="D31" s="53">
-        <v>50</v>
-      </c>
-      <c r="E31" s="54" t="s">
-        <v>4</v>
-      </c>
-      <c r="F31" s="36" t="s">
-        <v>53</v>
-      </c>
+      <c r="D31" s="53"/>
+      <c r="E31" s="54"/>
+      <c r="F31" s="36"/>
       <c r="G31" s="18"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A32" s="8">
+      <c r="A32" s="8" t="str">
         <f>IF(ISBLANK(B32),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B32))</f>
-        <v>40</v>
-      </c>
-      <c r="B32" s="47">
-        <v>45569</v>
-      </c>
-      <c r="C32" s="48">
-        <v>1</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B32" s="47"/>
+      <c r="C32" s="48"/>
       <c r="D32" s="49"/>
-      <c r="E32" s="50" t="s">
-        <v>3</v>
-      </c>
-      <c r="F32" s="55" t="s">
-        <v>54</v>
-      </c>
+      <c r="E32" s="50"/>
+      <c r="F32" s="55"/>
       <c r="G32" s="16"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A33" s="17">
+      <c r="A33" s="17" t="str">
         <f>IF(ISBLANK(B33),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B33))</f>
-        <v>40</v>
-      </c>
-      <c r="B33" s="51">
-        <v>45570</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B33" s="51"/>
       <c r="C33" s="52"/>
-      <c r="D33" s="53">
-        <v>30</v>
-      </c>
-      <c r="E33" s="54" t="s">
-        <v>22</v>
-      </c>
-      <c r="F33" s="36" t="s">
-        <v>55</v>
-      </c>
+      <c r="D33" s="53"/>
+      <c r="E33" s="54"/>
+      <c r="F33" s="36"/>
       <c r="G33" s="18"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A34" s="8">
+      <c r="A34" s="8" t="str">
         <f>IF(ISBLANK(B34),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B34))</f>
-        <v>40</v>
-      </c>
-      <c r="B34" s="47">
-        <v>45570</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B34" s="47"/>
       <c r="C34" s="48"/>
-      <c r="D34" s="49">
-        <v>20</v>
-      </c>
-      <c r="E34" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="F34" s="36" t="s">
-        <v>56</v>
-      </c>
+      <c r="D34" s="49"/>
+      <c r="E34" s="50"/>
+      <c r="F34" s="36"/>
       <c r="G34" s="16"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A35" s="17">
+      <c r="A35" s="17" t="str">
         <f>IF(ISBLANK(B35),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B35))</f>
-        <v>40</v>
-      </c>
-      <c r="B35" s="51">
-        <v>45570</v>
-      </c>
-      <c r="C35" s="52">
-        <v>2</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B35" s="51"/>
+      <c r="C35" s="52"/>
       <c r="D35" s="53"/>
-      <c r="E35" s="54" t="s">
-        <v>4</v>
-      </c>
-      <c r="F35" s="37" t="s">
-        <v>57</v>
-      </c>
+      <c r="E35" s="54"/>
+      <c r="F35" s="37"/>
       <c r="G35" s="18"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A36" s="8">
+      <c r="A36" s="8" t="str">
         <f>IF(ISBLANK(B36),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B36))</f>
-        <v>41</v>
-      </c>
-      <c r="B36" s="47">
-        <v>45576</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B36" s="47"/>
       <c r="C36" s="48"/>
-      <c r="D36" s="49">
-        <v>10</v>
-      </c>
-      <c r="E36" s="50" t="s">
-        <v>7</v>
-      </c>
-      <c r="F36" s="36" t="s">
-        <v>58</v>
-      </c>
+      <c r="D36" s="49"/>
+      <c r="E36" s="50"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="16"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A37" s="17">
+      <c r="A37" s="17" t="str">
         <f>IF(ISBLANK(B37),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B37))</f>
-        <v>41</v>
-      </c>
-      <c r="B37" s="51">
-        <v>45576</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B37" s="51"/>
       <c r="C37" s="52"/>
-      <c r="D37" s="53">
-        <v>10</v>
-      </c>
-      <c r="E37" s="54" t="s">
-        <v>6</v>
-      </c>
-      <c r="F37" s="36" t="s">
-        <v>59</v>
-      </c>
+      <c r="D37" s="53"/>
+      <c r="E37" s="54"/>
+      <c r="F37" s="36"/>
       <c r="G37" s="18"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A38" s="8">
+      <c r="A38" s="8" t="str">
         <f>IF(ISBLANK(B38),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B38))</f>
-        <v>41</v>
-      </c>
-      <c r="B38" s="47">
-        <v>45576</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B38" s="47"/>
       <c r="C38" s="48"/>
-      <c r="D38" s="49">
-        <v>15</v>
-      </c>
-      <c r="E38" s="50" t="s">
-        <v>7</v>
-      </c>
-      <c r="F38" s="36" t="s">
-        <v>60</v>
-      </c>
+      <c r="D38" s="49"/>
+      <c r="E38" s="50"/>
+      <c r="F38" s="36"/>
       <c r="G38" s="16"/>
     </row>
     <row r="39" spans="1:7" ht="16.5" x14ac:dyDescent="0.5">
-      <c r="A39" s="17">
+      <c r="A39" s="17" t="str">
         <f>IF(ISBLANK(B39),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B39))</f>
-        <v>41</v>
-      </c>
-      <c r="B39" s="51">
-        <v>45576</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B39" s="51"/>
       <c r="C39" s="52"/>
-      <c r="D39" s="53">
-        <v>5</v>
-      </c>
-      <c r="E39" s="54" t="s">
-        <v>6</v>
-      </c>
-      <c r="F39" s="56" t="s">
-        <v>61</v>
-      </c>
+      <c r="D39" s="53"/>
+      <c r="E39" s="54"/>
+      <c r="F39" s="56"/>
       <c r="G39" s="18"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A40" s="8">
+      <c r="A40" s="8" t="str">
         <f>IF(ISBLANK(B40),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B40))</f>
-        <v>41</v>
-      </c>
-      <c r="B40" s="47">
-        <v>45576</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B40" s="47"/>
       <c r="C40" s="48"/>
-      <c r="D40" s="49">
-        <v>10</v>
-      </c>
-      <c r="E40" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="F40" s="36" t="s">
-        <v>62</v>
-      </c>
+      <c r="D40" s="49"/>
+      <c r="E40" s="50"/>
+      <c r="F40" s="36"/>
       <c r="G40" s="16"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A41" s="17">
+      <c r="A41" s="17" t="str">
         <f>IF(ISBLANK(B41),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B41))</f>
-        <v>41</v>
-      </c>
-      <c r="B41" s="51">
-        <v>45576</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B41" s="51"/>
       <c r="C41" s="52"/>
-      <c r="D41" s="53">
-        <v>10</v>
-      </c>
-      <c r="E41" s="54" t="s">
-        <v>6</v>
-      </c>
-      <c r="F41" s="36" t="s">
-        <v>63</v>
-      </c>
+      <c r="D41" s="53"/>
+      <c r="E41" s="54"/>
+      <c r="F41" s="36"/>
       <c r="G41" s="18"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A42" s="8">
+      <c r="A42" s="8" t="str">
         <f>IF(ISBLANK(B42),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B42))</f>
-        <v>41</v>
-      </c>
-      <c r="B42" s="47">
-        <v>45576</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B42" s="47"/>
       <c r="C42" s="48"/>
-      <c r="D42" s="49">
-        <v>15</v>
-      </c>
-      <c r="E42" s="50" t="s">
-        <v>22</v>
-      </c>
-      <c r="F42" s="36" t="s">
-        <v>64</v>
-      </c>
+      <c r="D42" s="49"/>
+      <c r="E42" s="50"/>
+      <c r="F42" s="36"/>
       <c r="G42" s="16"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A43" s="17">
+      <c r="A43" s="17" t="str">
         <f>IF(ISBLANK(B43),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B43))</f>
-        <v>41</v>
-      </c>
-      <c r="B43" s="51">
-        <v>45576</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B43" s="51"/>
       <c r="C43" s="52"/>
-      <c r="D43" s="53">
-        <v>30</v>
-      </c>
-      <c r="E43" s="54" t="s">
-        <v>6</v>
-      </c>
-      <c r="F43" s="36" t="s">
-        <v>65</v>
-      </c>
+      <c r="D43" s="53"/>
+      <c r="E43" s="54"/>
+      <c r="F43" s="36"/>
       <c r="G43" s="18"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A44" s="8">
+      <c r="A44" s="8" t="str">
         <f>IF(ISBLANK(B44),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B44))</f>
-        <v>41</v>
-      </c>
-      <c r="B44" s="47">
-        <v>45576</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B44" s="47"/>
       <c r="C44" s="48"/>
-      <c r="D44" s="49">
-        <v>10</v>
-      </c>
-      <c r="E44" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="F44" s="36" t="s">
-        <v>66</v>
-      </c>
+      <c r="D44" s="49"/>
+      <c r="E44" s="50"/>
+      <c r="F44" s="36"/>
       <c r="G44" s="16"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A45" s="17">
+      <c r="A45" s="17" t="str">
         <f>IF(ISBLANK(B45),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B45))</f>
-        <v>41</v>
-      </c>
-      <c r="B45" s="51">
-        <v>45576</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B45" s="51"/>
       <c r="C45" s="52"/>
-      <c r="D45" s="53">
-        <v>10</v>
-      </c>
-      <c r="E45" s="54" t="s">
-        <v>4</v>
-      </c>
-      <c r="F45" s="36" t="s">
-        <v>67</v>
-      </c>
+      <c r="D45" s="53"/>
+      <c r="E45" s="54"/>
+      <c r="F45" s="36"/>
       <c r="G45" s="18"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A46" s="8">
+      <c r="A46" s="8" t="str">
         <f>IF(ISBLANK(B46),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B46))</f>
-        <v>41</v>
-      </c>
-      <c r="B46" s="47">
-        <v>45578</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B46" s="47"/>
       <c r="C46" s="48"/>
-      <c r="D46" s="49">
-        <v>20</v>
-      </c>
-      <c r="E46" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="F46" s="36" t="s">
-        <v>68</v>
-      </c>
+      <c r="D46" s="49"/>
+      <c r="E46" s="50"/>
+      <c r="F46" s="36"/>
       <c r="G46" s="16"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A47" s="17">
+      <c r="A47" s="17" t="str">
         <f>IF(ISBLANK(B47),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B47))</f>
-        <v>41</v>
-      </c>
-      <c r="B47" s="51">
-        <v>45578</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B47" s="51"/>
       <c r="C47" s="52"/>
-      <c r="D47" s="53">
-        <v>15</v>
-      </c>
-      <c r="E47" s="54" t="s">
-        <v>4</v>
-      </c>
-      <c r="F47" s="36" t="s">
-        <v>69</v>
-      </c>
+      <c r="D47" s="53"/>
+      <c r="E47" s="54"/>
+      <c r="F47" s="36"/>
       <c r="G47" s="18"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A48" s="8">
+      <c r="A48" s="8" t="str">
         <f>IF(ISBLANK(B48),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B48))</f>
-        <v>43</v>
-      </c>
-      <c r="B48" s="47">
-        <v>45586</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B48" s="47"/>
       <c r="C48" s="48"/>
-      <c r="D48" s="49">
-        <v>50</v>
-      </c>
-      <c r="E48" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="F48" s="36" t="s">
-        <v>70</v>
-      </c>
+      <c r="D48" s="49"/>
+      <c r="E48" s="50"/>
+      <c r="F48" s="36"/>
       <c r="G48" s="16"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A49" s="17">
+      <c r="A49" s="17" t="str">
         <f>IF(ISBLANK(B49),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B49))</f>
-        <v>43</v>
-      </c>
-      <c r="B49" s="51">
-        <v>45586</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B49" s="51"/>
       <c r="C49" s="52"/>
-      <c r="D49" s="53">
-        <v>20</v>
-      </c>
-      <c r="E49" s="54" t="s">
-        <v>4</v>
-      </c>
-      <c r="F49" s="36" t="s">
-        <v>71</v>
-      </c>
+      <c r="D49" s="53"/>
+      <c r="E49" s="54"/>
+      <c r="F49" s="36"/>
       <c r="G49" s="18"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A50" s="8">
+      <c r="A50" s="8" t="str">
         <f>IF(ISBLANK(B50),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B50))</f>
-        <v>43</v>
-      </c>
-      <c r="B50" s="47">
-        <v>45587</v>
-      </c>
-      <c r="C50" s="48">
-        <v>1</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B50" s="47"/>
+      <c r="C50" s="48"/>
       <c r="D50" s="49"/>
-      <c r="E50" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="F50" s="36" t="s">
-        <v>72</v>
-      </c>
+      <c r="E50" s="50"/>
+      <c r="F50" s="36"/>
       <c r="G50" s="16"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A51" s="17">
+      <c r="A51" s="17" t="str">
         <f>IF(ISBLANK(B51),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B51))</f>
-        <v>43</v>
-      </c>
-      <c r="B51" s="51">
-        <v>45587</v>
-      </c>
-      <c r="C51" s="52">
-        <v>2</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B51" s="51"/>
+      <c r="C51" s="52"/>
       <c r="D51" s="53"/>
-      <c r="E51" s="54" t="s">
-        <v>4</v>
-      </c>
-      <c r="F51" s="36" t="s">
-        <v>73</v>
-      </c>
+      <c r="E51" s="54"/>
+      <c r="F51" s="36"/>
       <c r="G51" s="18"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A52" s="8">
+      <c r="A52" s="8" t="str">
         <f>IF(ISBLANK(B52),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B52))</f>
-        <v>43</v>
-      </c>
-      <c r="B52" s="47">
-        <v>45588</v>
-      </c>
-      <c r="C52" s="48">
-        <v>1</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B52" s="47"/>
+      <c r="C52" s="48"/>
       <c r="D52" s="49"/>
-      <c r="E52" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="F52" s="36" t="s">
-        <v>74</v>
-      </c>
+      <c r="E52" s="50"/>
+      <c r="F52" s="36"/>
       <c r="G52" s="16"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A53" s="17">
+      <c r="A53" s="17" t="str">
         <f>IF(ISBLANK(B53),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B53))</f>
-        <v>43</v>
-      </c>
-      <c r="B53" s="51">
-        <v>45588</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B53" s="51"/>
       <c r="C53" s="52"/>
-      <c r="D53" s="53">
-        <v>0</v>
-      </c>
-      <c r="E53" s="54" t="s">
-        <v>4</v>
-      </c>
-      <c r="F53" s="36" t="s">
-        <v>75</v>
-      </c>
+      <c r="D53" s="53"/>
+      <c r="E53" s="54"/>
+      <c r="F53" s="36"/>
       <c r="G53" s="18"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A54" s="8">
+      <c r="A54" s="8" t="str">
         <f>IF(ISBLANK(B54),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B54))</f>
-        <v>43</v>
-      </c>
-      <c r="B54" s="47">
-        <v>45588</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B54" s="47"/>
       <c r="C54" s="48"/>
-      <c r="D54" s="49">
-        <v>5</v>
-      </c>
-      <c r="E54" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="F54" s="36" t="s">
-        <v>76</v>
-      </c>
+      <c r="D54" s="49"/>
+      <c r="E54" s="50"/>
+      <c r="F54" s="36"/>
       <c r="G54" s="16"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A55" s="17">
+      <c r="A55" s="17" t="str">
         <f>IF(ISBLANK(B55),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B55))</f>
-        <v>43</v>
-      </c>
-      <c r="B55" s="51">
-        <v>45588</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B55" s="51"/>
       <c r="C55" s="52"/>
-      <c r="D55" s="53">
-        <v>10</v>
-      </c>
-      <c r="E55" s="54" t="s">
-        <v>4</v>
-      </c>
-      <c r="F55" s="36" t="s">
-        <v>77</v>
-      </c>
+      <c r="D55" s="53"/>
+      <c r="E55" s="54"/>
+      <c r="F55" s="36"/>
       <c r="G55" s="18"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.5">
@@ -9127,7 +8584,7 @@
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C4,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="B4">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C4,'Journal de travail'!$D$7:$D$532)</f>
@@ -9139,17 +8596,17 @@
       </c>
       <c r="D4" s="34">
         <f>(A4+B4)/1440</f>
-        <v>4.1666666666666664E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>480</v>
+        <v>0</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>575</v>
+        <v>0</v>
       </c>
       <c r="C5" s="42" t="str">
         <f>'Journal de travail'!M9</f>
@@ -9157,7 +8614,7 @@
       </c>
       <c r="D5" s="34">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.73263888888888884</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -9185,7 +8642,7 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>95</v>
+        <v>0</v>
       </c>
       <c r="C7" s="28" t="str">
         <f>'Journal de travail'!M11</f>
@@ -9193,7 +8650,7 @@
       </c>
       <c r="D7" s="34">
         <f t="shared" si="0"/>
-        <v>6.5972222222222224E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -9203,7 +8660,7 @@
       </c>
       <c r="B8">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C8,'Journal de travail'!$D$7:$D$532)</f>
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="C8" s="29" t="str">
         <f>'Journal de travail'!M12</f>
@@ -9211,7 +8668,7 @@
       </c>
       <c r="D8" s="34">
         <f t="shared" si="0"/>
-        <v>3.125E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -9249,7 +8706,7 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B11">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C11,'Journal de travail'!$D$7:$D$532)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="C11" s="40" t="str">
         <f>'Journal de travail'!M15</f>
@@ -9257,7 +8714,7 @@
       </c>
       <c r="D11" s="34">
         <f t="shared" si="0"/>
-        <v>6.9444444444444448E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -9266,7 +8723,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>0.9409722222222221</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -9280,26 +8737,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9522,10 +8959,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9542,20 +9010,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Doc: Update journal de travail temp
</commit_message>
<xml_diff>
--- a/Docs/Journal-de-Travail_Temp.xlsx
+++ b/Docs/Journal-de-Travail_Temp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BILEL\Documents\PlotThatLine\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB7A3AB-6114-432A-A4F1-DF6CA92E2768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26DBAF5A-59F8-4756-A506-E88BFA5E73F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>30.08.2024  au 01.11.2024</t>
+  </si>
+  <si>
+    <t>Fix permettant de ne plus réafficher toutes les équipes en cas de filtre sur un jour</t>
   </si>
 </sst>
 </file>
@@ -1062,7 +1065,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>6.9444444444444441E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1993,7 +1996,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -2046,7 +2049,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 0 heurs 0 minutes</v>
+        <v>0 jours 0 heurs 10 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2065,11 +2068,11 @@
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2104,15 +2107,23 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.5">
-      <c r="A7" s="14" t="str">
+      <c r="A7" s="14">
         <f>IF(ISBLANK(B7),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B7))</f>
-        <v/>
-      </c>
-      <c r="B7" s="43"/>
+        <v>43</v>
+      </c>
+      <c r="B7" s="43">
+        <v>45589</v>
+      </c>
       <c r="C7" s="44"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="37"/>
+      <c r="D7" s="45">
+        <v>10</v>
+      </c>
+      <c r="E7" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="37" t="s">
+        <v>29</v>
+      </c>
       <c r="G7" s="15"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.5">
@@ -8606,7 +8617,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C5" s="42" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8614,7 +8625,7 @@
       </c>
       <c r="D5" s="34">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0</v>
+        <v>6.9444444444444441E-3</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -8723,7 +8734,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>0</v>
+        <v>6.9444444444444441E-3</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
Doc: Update journal travail temp
</commit_message>
<xml_diff>
--- a/Docs/Journal-de-Travail_Temp.xlsx
+++ b/Docs/Journal-de-Travail_Temp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BILEL\Documents\PlotThatLine\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D321B09A-4DEE-47CA-9146-87F59BB2B6A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F9CAE8-1187-42F6-9EB7-DF684818F896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -155,6 +155,9 @@
   </si>
   <si>
     <t>Ajout d'un test unitaire qui vérifie que suite a la méthode createGraph le graph n'est pas vide</t>
+  </si>
+  <si>
+    <t>Ajout d'un test unitaire sur la méthode loadFile</t>
   </si>
 </sst>
 </file>
@@ -1102,7 +1105,7 @@
                   <c:v>4.1666666666666664E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.7361111111111112E-2</c:v>
+                  <c:v>2.7777777777777776E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2.4305555555555556E-2</c:v>
@@ -2028,7 +2031,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O532"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
@@ -2083,7 +2086,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 2 heurs 15 minutes</v>
+        <v>0 jours 2 heurs 30 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2102,11 +2105,11 @@
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>135</v>
+        <v>150</v>
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>135</v>
+        <v>150</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2408,15 +2411,23 @@
       </c>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="17" t="str">
+      <c r="A17" s="17">
         <f>IF(ISBLANK(B17),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B17))</f>
-        <v/>
-      </c>
-      <c r="B17" s="51"/>
+        <v>44</v>
+      </c>
+      <c r="B17" s="51">
+        <v>45594</v>
+      </c>
       <c r="C17" s="52"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="37"/>
+      <c r="D17" s="53">
+        <v>15</v>
+      </c>
+      <c r="E17" s="54" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="37" t="s">
+        <v>38</v>
+      </c>
       <c r="G17" s="18"/>
       <c r="O17">
         <v>45</v>
@@ -8733,7 +8744,7 @@
       </c>
       <c r="B6">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C6,'Journal de travail'!$D$7:$D$532)</f>
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="C6" s="27" t="str">
         <f>'Journal de travail'!M10</f>
@@ -8741,7 +8752,7 @@
       </c>
       <c r="D6" s="34">
         <f t="shared" si="0"/>
-        <v>1.7361111111111112E-2</v>
+        <v>2.7777777777777776E-2</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -8832,7 +8843,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>9.375E-2</v>
+        <v>0.10416666666666666</v>
       </c>
     </row>
     <row r="14" spans="1:4">

</xml_diff>

<commit_message>
Doc Update journal de travail temp
</commit_message>
<xml_diff>
--- a/Docs/Journal-de-Travail_Temp.xlsx
+++ b/Docs/Journal-de-Travail_Temp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BILEL\Documents\PlotThatLine\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB3CAA3-3228-4A76-B5C0-097FF4A4323F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A42A7211-54AD-4AAA-8B21-794B1F2EE371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -2039,7 +2039,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>

</xml_diff>